<commit_message>
added multi-scene capability to multi-block fixed multi_block result names
</commit_message>
<xml_diff>
--- a/Projects/GMIUS/Data/Mexican GMI KPI template v0.3.xlsx
+++ b/Projects/GMIUS/Data/Mexican GMI KPI template v0.3.xlsx
@@ -287,7 +287,7 @@
     <t xml:space="preserve">&lt;5, 5, 6, 7, 8, &gt;=9</t>
   </si>
   <si>
-    <t xml:space="preserve">Taco, Enchilada Sauce and Cooking Sauce together, Taco and enchilada sauce together, not cooking sauce, Taco and cooking sauce together, not enchilada sauce, Enchilada and Cookie sauce together, not taco sauce, None shelved together</t>
+    <t xml:space="preserve">Taco, Enchilada Sauce and Cooking Sauce together; Taco &amp; Enchilada Sauce together, not Cooking Sauce; Taco &amp; Cooking Sauce together, not Enchilada Sauce; Enchilada &amp; Cooking Sauce together, not Taco Sauce; None shelved together</t>
   </si>
   <si>
     <t xml:space="preserve">Blocked, Not Blocked</t>
@@ -829,7 +829,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -1299,8 +1299,8 @@
   </sheetPr>
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -1488,7 +1488,7 @@
         <v>86</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>11</v>

</xml_diff>